<commit_message>
Update database, add k-value textbox
Update database following the weekend's matches, added k-value input.
Cycles through multiple values if value <= 0.
</commit_message>
<xml_diff>
--- a/Spreadsheets/hurling.xlsx
+++ b/Spreadsheets/hurling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7188" yWindow="6288" windowWidth="7020" windowHeight="6312" activeTab="1"/>
+    <workbookView xWindow="7188" yWindow="6288" windowWidth="7020" windowHeight="6312"/>
   </bookViews>
   <sheets>
     <sheet name="teams" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="148">
   <si>
     <t>Antrim</t>
   </si>
@@ -458,6 +458,9 @@
   <si>
     <t>St. Patrick's Park Donagh</t>
   </si>
+  <si>
+    <t>Current Rating (k =24)</t>
+  </si>
 </sst>
 </file>
 
@@ -823,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -832,6 +835,7 @@
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1">
@@ -844,6 +848,9 @@
       <c r="C1" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
@@ -855,6 +862,9 @@
       <c r="C2">
         <v>1775</v>
       </c>
+      <c r="D2">
+        <v>1610</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -865,6 +875,9 @@
       </c>
       <c r="C3">
         <v>1450</v>
+      </c>
+      <c r="D3">
+        <v>1460</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -877,7 +890,9 @@
       <c r="C4">
         <v>1700</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>1611</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
@@ -889,7 +904,9 @@
       <c r="C5">
         <v>1850</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>1938</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
@@ -901,7 +918,9 @@
       <c r="C6">
         <v>1975</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>1908</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -913,7 +932,9 @@
       <c r="C7">
         <v>1650</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>1479</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
@@ -925,7 +946,9 @@
       <c r="C8">
         <v>1300</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>1307</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
@@ -937,7 +960,9 @@
       <c r="C9">
         <v>1575</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>1555</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
@@ -949,7 +974,9 @@
       <c r="C10">
         <v>1875</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>1885</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
@@ -961,7 +988,9 @@
       <c r="C11">
         <v>1250</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>1208</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -973,7 +1002,9 @@
       <c r="C12">
         <v>1375</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>1343</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
@@ -985,7 +1016,9 @@
       <c r="C13">
         <v>1900</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>1898</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -997,7 +1030,9 @@
       <c r="C14">
         <v>1625</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>1737</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
@@ -1009,7 +1044,9 @@
       <c r="C15">
         <v>1550</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>1556</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
@@ -1021,7 +1058,9 @@
       <c r="C16">
         <v>2000</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>2074</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
@@ -1033,7 +1072,9 @@
       <c r="C17">
         <v>1000</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>945</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
@@ -1045,7 +1086,9 @@
       <c r="C18">
         <v>1725</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2">
+        <v>1637</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
@@ -1057,7 +1100,9 @@
       <c r="C19">
         <v>1200</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>1082</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
@@ -1069,7 +1114,9 @@
       <c r="C20">
         <v>1825</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>1885</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
@@ -1081,7 +1128,9 @@
       <c r="C21">
         <v>1475</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>1513</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
@@ -1093,7 +1142,9 @@
       <c r="C22">
         <v>1175</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>1222</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
@@ -1105,7 +1156,9 @@
       <c r="C23">
         <v>1350</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>1307</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
@@ -1117,7 +1170,9 @@
       <c r="C24">
         <v>1500</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>1465</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
@@ -1129,7 +1184,9 @@
       <c r="C25">
         <v>1525</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>1564</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
@@ -1141,7 +1198,9 @@
       <c r="C26">
         <v>1400</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>1297</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
@@ -1153,7 +1212,9 @@
       <c r="C27">
         <v>1800</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>1726</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
@@ -1165,7 +1226,9 @@
       <c r="C28">
         <v>1425</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>1459</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
@@ -1177,7 +1240,9 @@
       <c r="C29">
         <v>1275</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>1122</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
@@ -1189,7 +1254,9 @@
       <c r="C30">
         <v>1950</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>1976</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
@@ -1201,7 +1268,9 @@
       <c r="C31">
         <v>1325</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>1367</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
@@ -1213,7 +1282,9 @@
       <c r="C32">
         <v>1225</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>1156</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
@@ -1225,7 +1296,9 @@
       <c r="C33">
         <v>1925</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>1970</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
@@ -1237,7 +1310,9 @@
       <c r="C34">
         <v>1675</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>1678</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
@@ -1249,7 +1324,9 @@
       <c r="C35">
         <v>1750</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>1772</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
@@ -1261,7 +1338,9 @@
       <c r="C36">
         <v>1600</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>1486</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
@@ -1273,6 +1352,9 @@
       <c r="C37">
         <v>0</v>
       </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
@@ -1284,9 +1366,12 @@
       <c r="C38">
         <v>0</v>
       </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C35">
+  <sortState ref="A2:D38">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1295,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N793"/>
+  <dimension ref="A1:N799"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A773" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -39027,7 +39112,7 @@
         <v>16</v>
       </c>
       <c r="K770" s="3">
-        <f t="shared" ref="K770:K793" si="50">IF(I770&gt;J770,1,(IF(I770&lt;J770,0,0.5)))</f>
+        <f t="shared" ref="K770:K799" si="50">IF(I770&gt;J770,1,(IF(I770&lt;J770,0,0.5)))</f>
         <v>0</v>
       </c>
       <c r="L770" s="3">
@@ -39043,7 +39128,7 @@
     </row>
     <row r="771" spans="1:14">
       <c r="A771" s="3">
-        <f t="shared" ref="A771:A793" si="51">A770+1</f>
+        <f t="shared" ref="A771:A799" si="51">A770+1</f>
         <v>770</v>
       </c>
       <c r="B771" s="4">
@@ -40166,6 +40251,300 @@
       </c>
       <c r="N793" s="3" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="794" spans="1:14">
+      <c r="A794" s="3">
+        <f t="shared" si="51"/>
+        <v>793</v>
+      </c>
+      <c r="B794" s="4">
+        <v>42547</v>
+      </c>
+      <c r="C794" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D794">
+        <v>5</v>
+      </c>
+      <c r="E794">
+        <v>17</v>
+      </c>
+      <c r="F794">
+        <v>4</v>
+      </c>
+      <c r="G794">
+        <v>21</v>
+      </c>
+      <c r="H794" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I794" s="3">
+        <f t="shared" ref="I794:I799" si="52">D794*3 + E794</f>
+        <v>32</v>
+      </c>
+      <c r="J794" s="3">
+        <f t="shared" ref="J794:J799" si="53">F794*3 + G794</f>
+        <v>33</v>
+      </c>
+      <c r="K794" s="3">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="L794" s="3">
+        <f>COUNTIF($K$2:K794, 0.5)/COUNT($K$2:K794)</f>
+        <v>6.0529634300126103E-2</v>
+      </c>
+      <c r="M794" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N794" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="795" spans="1:14">
+      <c r="A795" s="3">
+        <f t="shared" si="51"/>
+        <v>794</v>
+      </c>
+      <c r="B795" s="4">
+        <v>42553</v>
+      </c>
+      <c r="C795" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D795">
+        <v>1</v>
+      </c>
+      <c r="E795">
+        <v>21</v>
+      </c>
+      <c r="F795">
+        <v>1</v>
+      </c>
+      <c r="G795">
+        <v>13</v>
+      </c>
+      <c r="H795" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I795" s="3">
+        <f t="shared" si="52"/>
+        <v>24</v>
+      </c>
+      <c r="J795" s="3">
+        <f t="shared" si="53"/>
+        <v>16</v>
+      </c>
+      <c r="K795" s="3">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="L795" s="3">
+        <f>COUNTIF($K$2:K795, 0.5)/COUNT($K$2:K795)</f>
+        <v>6.0453400503778336E-2</v>
+      </c>
+      <c r="M795" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N795" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="796" spans="1:14">
+      <c r="A796" s="3">
+        <f t="shared" si="51"/>
+        <v>795</v>
+      </c>
+      <c r="B796" s="4">
+        <v>42553</v>
+      </c>
+      <c r="C796" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D796">
+        <v>0</v>
+      </c>
+      <c r="E796">
+        <v>18</v>
+      </c>
+      <c r="F796">
+        <v>1</v>
+      </c>
+      <c r="G796">
+        <v>24</v>
+      </c>
+      <c r="H796" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I796" s="3">
+        <f t="shared" si="52"/>
+        <v>18</v>
+      </c>
+      <c r="J796" s="3">
+        <f t="shared" si="53"/>
+        <v>27</v>
+      </c>
+      <c r="K796" s="3">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="L796" s="3">
+        <f>COUNTIF($K$2:K796, 0.5)/COUNT($K$2:K796)</f>
+        <v>6.0377358490566038E-2</v>
+      </c>
+      <c r="M796" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N796" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="797" spans="1:14">
+      <c r="A797" s="3">
+        <f t="shared" si="51"/>
+        <v>796</v>
+      </c>
+      <c r="B797" s="4">
+        <v>42553</v>
+      </c>
+      <c r="C797" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D797">
+        <v>5</v>
+      </c>
+      <c r="E797">
+        <v>32</v>
+      </c>
+      <c r="F797">
+        <v>0</v>
+      </c>
+      <c r="G797">
+        <v>12</v>
+      </c>
+      <c r="H797" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I797" s="3">
+        <f t="shared" si="52"/>
+        <v>47</v>
+      </c>
+      <c r="J797" s="3">
+        <f t="shared" si="53"/>
+        <v>12</v>
+      </c>
+      <c r="K797" s="3">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="L797" s="3">
+        <f>COUNTIF($K$2:K797, 0.5)/COUNT($K$2:K797)</f>
+        <v>6.030150753768844E-2</v>
+      </c>
+      <c r="M797" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N797" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="798" spans="1:14">
+      <c r="A798" s="3">
+        <f t="shared" si="51"/>
+        <v>797</v>
+      </c>
+      <c r="B798" s="4">
+        <v>42553</v>
+      </c>
+      <c r="C798" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D798">
+        <v>1</v>
+      </c>
+      <c r="E798">
+        <v>26</v>
+      </c>
+      <c r="F798">
+        <v>1</v>
+      </c>
+      <c r="G798">
+        <v>23</v>
+      </c>
+      <c r="H798" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I798" s="3">
+        <f t="shared" si="52"/>
+        <v>29</v>
+      </c>
+      <c r="J798" s="3">
+        <f t="shared" si="53"/>
+        <v>26</v>
+      </c>
+      <c r="K798" s="3">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="L798" s="3">
+        <f>COUNTIF($K$2:K798, 0.5)/COUNT($K$2:K798)</f>
+        <v>6.0225846925972396E-2</v>
+      </c>
+      <c r="M798" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N798" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="799" spans="1:14">
+      <c r="A799" s="3">
+        <f t="shared" si="51"/>
+        <v>798</v>
+      </c>
+      <c r="B799" s="4">
+        <v>42554</v>
+      </c>
+      <c r="C799" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D799">
+        <v>0</v>
+      </c>
+      <c r="E799">
+        <v>22</v>
+      </c>
+      <c r="F799">
+        <v>1</v>
+      </c>
+      <c r="G799">
+        <v>26</v>
+      </c>
+      <c r="H799" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I799" s="3">
+        <f t="shared" si="52"/>
+        <v>22</v>
+      </c>
+      <c r="J799" s="3">
+        <f t="shared" si="53"/>
+        <v>29</v>
+      </c>
+      <c r="K799" s="3">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="L799" s="3">
+        <f>COUNTIF($K$2:K799, 0.5)/COUNT($K$2:K799)</f>
+        <v>6.0150375939849621E-2</v>
+      </c>
+      <c r="M799" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N799" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>